<commit_message>
Created C3DC testcases for phs002599
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs002504_SexAtBirth-Male.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs002504_SexAtBirth-Male.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/C3DC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-09-25-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A9A9E6-89A5-5E49-B8BA-032FD6987EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E5A3F0-7B52-1A4B-8FA8-0E8A2BB567BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-36420" yWindow="-1860" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,35 +183,6 @@
 LIMIT 100;</t>
   </si>
   <si>
-    <t>SELECT
-    DISTINCT prt.participant_id AS "Participant Id",
-    trt.treatment_id AS "Treatment Id",
-    trt.age_at_treatment_start AS "Age at Treatment Start",
-    trt.age_at_treatment_end AS "Age at Treatment End",
-    trt.treatment_type AS "Treatment Type",
-    CONCAT('[', REPLACE(trt.treatment_agent, ';', ', '), ']') AS "Treatment Agent",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs002504' AND prt.sex_at_birth = 'Male'
-ORDER BY 
-    trt.treatment_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SELECT DISTINCT
     prt.participant_id AS "Participant Id",
     trr.treatment_response_id AS "Treatment Response Id",
@@ -276,16 +247,81 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs002504' AND prt.sex_at_birth = 'Male';</t>
+    std.dbgap_accession = 'phs002504' AND prt.sex_at_birth = 'Male'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT
+    DISTINCT prt.participant_id AS "Participant Id",
+    trt.treatment_id AS "Treatment Id",
+    CASE 
+    WHEN trt.age_at_treatment_start = -999 THEN 'Not Reported'
+    WHEN trt.age_at_treatment_start &gt;= 1000 THEN 
+        substr(trt.age_at_treatment_start, 1, length(trt.age_at_treatment_start) - 3) || ',' || substr(trt.age_at_treatment_start, -3)
+    ELSE 
+        trt.age_at_treatment_start 
+END AS "Age at Treatment Start",
+    CASE 
+    WHEN trt.age_at_treatment_end = -999 THEN 'Not Reported'
+    WHEN trt.age_at_treatment_end &gt;= 1000 THEN 
+        substr(trt.age_at_treatment_end, 1, length(trt.age_at_treatment_end) - 3) || ',' || substr(trt.age_at_treatment_end, -3)
+    ELSE 
+        trt.age_at_treatment_end 
+END AS "Age at Treatment End",
+    trt.treatment_type AS "Treatment Type",
+    CONCAT(REPLACE(trt.treatment_agent, ';', ', ')) AS "Treatment Agent",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002504' AND prt.sex_at_birth = 'Male'
+ORDER BY 
+    trt.treatment_id ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -345,11 +381,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -678,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -712,10 +757,10 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -729,7 +774,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -737,7 +782,7 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2"/>
@@ -746,8 +791,8 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -756,7 +801,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -764,8 +809,8 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -777,7 +822,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>